<commit_message>
Data driven test case completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/VehicleInsuranceCalculator_TestData.xlsx
+++ b/src/test/resources/testData/VehicleInsuranceCalculator_TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Workspace\Java_Training.InsuranceCalculator1\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C689B8-4E52-4707-8307-FAC94132FA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InsurancePremium" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>TC No</t>
   </si>
@@ -120,15 +126,6 @@
     <t>Ultimate</t>
   </si>
   <si>
-    <t>5.000.000,00</t>
-  </si>
-  <si>
-    <t>20.000.000,00</t>
-  </si>
-  <si>
-    <t>3.000.000,00</t>
-  </si>
-  <si>
     <t>Partial Coverage</t>
   </si>
   <si>
@@ -184,16 +181,37 @@
   </si>
   <si>
     <t>Verify Insurance Premium for Audi Moped</t>
+  </si>
+  <si>
+    <t>04/09/2019</t>
+  </si>
+  <si>
+    <t>04/09/2001</t>
+  </si>
+  <si>
+    <t>04/09/1989</t>
+  </si>
+  <si>
+    <t>12/12/1989</t>
+  </si>
+  <si>
+    <t>12/12/1977</t>
+  </si>
+  <si>
+    <t>12/12/1956</t>
+  </si>
+  <si>
+    <t>06/15/2023</t>
+  </si>
+  <si>
+    <t>3000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,15 +264,23 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -301,7 +327,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,9 +359,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,6 +411,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -542,14 +604,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -580,93 +642,93 @@
     <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,8 +747,8 @@
       <c r="F2">
         <v>666</v>
       </c>
-      <c r="G2" s="2">
-        <v>43564</v>
+      <c r="G2" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -698,43 +760,43 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
         <v>46</v>
-      </c>
-      <c r="M2" s="2">
-        <v>32854</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O2" t="s">
-        <v>49</v>
       </c>
       <c r="P2">
         <v>444061</v>
       </c>
       <c r="Q2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
-        <v>45</v>
-      </c>
-      <c r="T2" s="2">
-        <v>44177</v>
-      </c>
-      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" t="s">
-        <v>37</v>
-      </c>
       <c r="W2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="X2" s="1">
         <v>238</v>
@@ -745,14 +807,14 @@
       <c r="Z2" s="1">
         <v>1376</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="2">
         <v>2621</v>
       </c>
       <c r="AB2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -771,8 +833,8 @@
       <c r="F3">
         <v>900</v>
       </c>
-      <c r="G3" s="2">
-        <v>36990</v>
+      <c r="G3" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -784,43 +846,43 @@
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="2">
-        <v>28471</v>
+        <v>43</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P3">
         <v>444061</v>
       </c>
       <c r="Q3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S3" t="s">
-        <v>45</v>
-      </c>
-      <c r="T3" s="2">
-        <v>46003</v>
-      </c>
-      <c r="U3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
         <v>35</v>
-      </c>
-      <c r="V3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" t="s">
-        <v>38</v>
       </c>
       <c r="X3" s="1">
         <v>238</v>
@@ -831,22 +893,22 @@
       <c r="Z3" s="1">
         <v>1379</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AA3" s="2">
         <v>2626</v>
       </c>
       <c r="AB3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
@@ -857,8 +919,8 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="2">
-        <v>32607</v>
+      <c r="G4" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -870,43 +932,43 @@
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="2">
-        <v>20801</v>
+        <v>43</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P4">
         <v>444061</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="2">
-        <v>46003</v>
-      </c>
-      <c r="U4" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="V4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="X4" s="1">
         <v>87</v>
@@ -931,24 +993,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>